<commit_message>
added companies, deals list
</commit_message>
<xml_diff>
--- a/companies.xlsx
+++ b/companies.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/32906c935fa0eb4f/models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="11_F25DC773A252ABDACC104889191A52245ADE58E6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C0715046-3912-46B7-BEBB-676B00BA6ACA}"/>
+  <xr:revisionPtr revIDLastSave="42" documentId="11_F25DC773A252ABDACC104889191A52245ADE58E6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B502B3FB-5D83-45A7-B72F-F881A1ED8B5E}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="4160" windowWidth="15530" windowHeight="12340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18790" yWindow="1390" windowWidth="19250" windowHeight="16940" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Companies" sheetId="1" r:id="rId1"/>
+    <sheet name="Public" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
     <t>Company Name</t>
   </si>
@@ -46,6 +47,153 @@
   </si>
   <si>
     <t>Optogenetics</t>
+  </si>
+  <si>
+    <t>Carbon Robotics</t>
+  </si>
+  <si>
+    <t>Micropep</t>
+  </si>
+  <si>
+    <t>Pyka</t>
+  </si>
+  <si>
+    <t>Ahold Delhaize</t>
+  </si>
+  <si>
+    <t>Purdue University</t>
+  </si>
+  <si>
+    <t>EarthOptics</t>
+  </si>
+  <si>
+    <t>Pairwise</t>
+  </si>
+  <si>
+    <t>Calyxia</t>
+  </si>
+  <si>
+    <t>Constructive Bio</t>
+  </si>
+  <si>
+    <t>Agrim</t>
+  </si>
+  <si>
+    <t>Pattern Ag</t>
+  </si>
+  <si>
+    <t>Solasta Bio</t>
+  </si>
+  <si>
+    <t>Vision Greens</t>
+  </si>
+  <si>
+    <t>Muon Space</t>
+  </si>
+  <si>
+    <t>Applied Carbon</t>
+  </si>
+  <si>
+    <t>InnerPlant</t>
+  </si>
+  <si>
+    <t>Arzeda</t>
+  </si>
+  <si>
+    <t>Colossal Laboratories &amp; Biosciences</t>
+  </si>
+  <si>
+    <t>Monarch Tractor</t>
+  </si>
+  <si>
+    <t>AgroSpheres</t>
+  </si>
+  <si>
+    <t>Standing Ovation</t>
+  </si>
+  <si>
+    <t>Dechra Pharmaceuticals</t>
+  </si>
+  <si>
+    <t>Produce Pay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create growing plans and underwrite preseason and operating loans. Marketplace for pre-orders of produce to happen before seed is planted. </t>
+  </si>
+  <si>
+    <t>Geography HQ/Hubs</t>
+  </si>
+  <si>
+    <t>LA, South America</t>
+  </si>
+  <si>
+    <t>Fintech, Agribusiness, E-commerce</t>
+  </si>
+  <si>
+    <t>Agco</t>
+  </si>
+  <si>
+    <t>Deere</t>
+  </si>
+  <si>
+    <t>GrainCorp</t>
+  </si>
+  <si>
+    <t>Nutrien</t>
+  </si>
+  <si>
+    <t>The Mosaic Company</t>
+  </si>
+  <si>
+    <t>Bunge Limited</t>
+  </si>
+  <si>
+    <t>Adecoagro</t>
+  </si>
+  <si>
+    <t>CF Industries Holdings Inc</t>
+  </si>
+  <si>
+    <t>ADM</t>
+  </si>
+  <si>
+    <t>Corteva</t>
+  </si>
+  <si>
+    <t>Nufarm</t>
+  </si>
+  <si>
+    <t>Scotts Miracle-Gro</t>
+  </si>
+  <si>
+    <t>Alico</t>
+  </si>
+  <si>
+    <t>Frieght Farms</t>
+  </si>
+  <si>
+    <t>Tyson</t>
+  </si>
+  <si>
+    <t>Mitsubishi-Food division</t>
+  </si>
+  <si>
+    <t>Toro</t>
+  </si>
+  <si>
+    <t>Farmer Mac</t>
+  </si>
+  <si>
+    <t>Ingredion Inc.</t>
+  </si>
+  <si>
+    <t>Lindsay Corporation</t>
+  </si>
+  <si>
+    <t>Bayer</t>
+  </si>
+  <si>
+    <t>FMC Crop</t>
   </si>
 </sst>
 </file>
@@ -90,9 +238,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -374,39 +523,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:D4"/>
+  <dimension ref="B2:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.36328125" customWidth="1"/>
-    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="3" max="3" width="54.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.36328125" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>0</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="D2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
@@ -414,12 +567,262 @@
         <v>6</v>
       </c>
     </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B20" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B21" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B23" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B27" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27" t="s">
+        <v>33</v>
+      </c>
+      <c r="D27" t="s">
+        <v>32</v>
+      </c>
+      <c r="E27" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1" display="https://agfundernews.com/biomanufacturing-game-changer-enduro-genetics-unveils-elegant-solution-to-declining-cell-productivity" xr:uid="{D52C37B8-6E45-4521-BBF2-BFC2CCA2188C}"/>
+    <hyperlink ref="E3" r:id="rId1" display="https://agfundernews.com/biomanufacturing-game-changer-enduro-genetics-unveils-elegant-solution-to-declining-cell-productivity" xr:uid="{D52C37B8-6E45-4521-BBF2-BFC2CCA2188C}"/>
     <hyperlink ref="B3" r:id="rId2" xr:uid="{CF9DA723-CD24-46AA-9A82-FBB0914ADC74}"/>
     <hyperlink ref="B4" r:id="rId3" xr:uid="{103022F1-3595-44A0-A586-B1FDF5686C22}"/>
+    <hyperlink ref="B27" r:id="rId4" xr:uid="{137576FA-FD27-474B-9A34-F2692E761C8B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDF9ECE1-1192-4F7A-A362-8E5BDDDCBEF2}">
+  <dimension ref="B2:B23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B17" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B18" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B19" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B20" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B21" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B22" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B23" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>